<commit_message>
Commit script 1 Richard
</commit_message>
<xml_diff>
--- a/Bleaching_MAP.xlsx
+++ b/Bleaching_MAP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\R\R-Git-Link\MATbleaching\MATbleaching\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63C4CF2B-09BF-49F2-B6B6-FDBEE2AB8A9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2480341-19F9-422D-97A0-9BD22BDE8115}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A064A2A8-AA0E-4D02-9B84-0DA3F01D5224}"/>
   </bookViews>
@@ -522,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28A24C5-3223-413F-B488-4E88C6609187}">
   <dimension ref="A1:G2881"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2367" workbookViewId="0">
-      <selection activeCell="G2377" sqref="G2377"/>
+    <sheetView tabSelected="1" topLeftCell="A435" workbookViewId="0">
+      <selection activeCell="G443" sqref="G443"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10548,7 +10548,7 @@
         <v>120.46459282421759</v>
       </c>
       <c r="G443" s="4">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="444" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>